<commit_message>
Reorganized iOS code - moved 4 receiversData update methods from Data.m to respective classes sentLinkViewController, receivedLinkViewController, and replyViewController. Added files from Android Development folder Pre-Launch To Do List.docx and Improvements (8-5).docx to git repo. Modified .gitignore to ignore all other files in folder.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/LinkMeUp Planning Doc.xlsx
+++ b/Documents/Logs and Planning/LinkMeUp Planning Doc.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="423">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -1357,9 +1357,6 @@
     <t>Go through (recent) Android code</t>
   </si>
   <si>
-    <t>Move local data update functions to data model (?)</t>
-  </si>
-  <si>
     <t>Scrolling autocomplete results hides keyboard</t>
   </si>
   <si>
@@ -1394,6 +1391,27 @@
   </si>
   <si>
     <t>Use Parse Analytics to track events/crashes</t>
+  </si>
+  <si>
+    <t>Updates</t>
+  </si>
+  <si>
+    <t>Renew/replace push certificates</t>
+  </si>
+  <si>
+    <t>Support iOS 9/Xcode 7</t>
+  </si>
+  <si>
+    <t>Replace for loops with for each loops</t>
+  </si>
+  <si>
+    <t>Make as many properties private as possible</t>
+  </si>
+  <si>
+    <t>Declare class for receiversData (NSDict subclass?)</t>
+  </si>
+  <si>
+    <t>Modularize local/server data update functions</t>
   </si>
 </sst>
 </file>
@@ -1533,7 +1551,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1564,12 +1582,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1580,7 +1592,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2499">
+  <cellStyleXfs count="2519">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4080,8 +4092,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4111,10 +4143,11 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2499">
+  <cellStyles count="2519">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5364,6 +5397,16 @@
     <cellStyle name="Followed Hyperlink" xfId="2494" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2496" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2498" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2500" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2502" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2504" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2514" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2516" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2518" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6613,6 +6656,16 @@
     <cellStyle name="Hyperlink" xfId="2493" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2495" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2497" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2499" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2501" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2503" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2513" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2515" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2517" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6947,8 +7000,8 @@
   </sheetPr>
   <dimension ref="A1:E178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7032,7 +7085,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>299</v>
@@ -7046,7 +7099,7 @@
         <v>43</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>284</v>
@@ -7060,7 +7113,7 @@
         <v>290</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -7074,7 +7127,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -7085,7 +7138,7 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>346</v>
@@ -7113,7 +7166,7 @@
         <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>344</v>
@@ -7122,7 +7175,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="C14" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -7134,9 +7187,11 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>412</v>
-      </c>
-      <c r="E15" s="10"/>
+        <v>411</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
@@ -7148,7 +7203,9 @@
       <c r="C16" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E16" s="10"/>
+      <c r="D16" s="24" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
@@ -7160,6 +7217,9 @@
       <c r="C17" s="18" t="s">
         <v>190</v>
       </c>
+      <c r="D17" s="24" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
@@ -7195,7 +7255,7 @@
         <v>364</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -7257,7 +7317,7 @@
         <v>53</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>356</v>
@@ -7271,7 +7331,7 @@
       <c r="B26" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="29" t="s">
         <v>47</v>
       </c>
       <c r="D26" s="20" t="s">
@@ -7314,15 +7374,15 @@
         <v>154</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>307</v>
+        <v>416</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="C30" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D30" s="24" t="s">
-        <v>327</v>
+      <c r="D30" s="27" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -7335,8 +7395,8 @@
       <c r="C31" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="D31" s="24" t="s">
-        <v>331</v>
+      <c r="D31" s="30" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -7349,6 +7409,9 @@
       <c r="C32" s="5" t="s">
         <v>158</v>
       </c>
+      <c r="D32" s="31" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
@@ -7385,7 +7448,7 @@
         <v>396</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E35" s="12"/>
     </row>
@@ -7543,7 +7606,7 @@
         <v>384</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E47" s="15"/>
     </row>
@@ -7596,8 +7659,8 @@
       <c r="C51" s="22" t="s">
         <v>386</v>
       </c>
-      <c r="D51" s="29" t="s">
-        <v>361</v>
+      <c r="D51" s="27" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -7611,7 +7674,7 @@
         <v>389</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>301</v>
+        <v>348</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -7625,7 +7688,7 @@
         <v>387</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -7633,7 +7696,7 @@
         <v>391</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -7646,9 +7709,6 @@
       <c r="C55" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="D55" s="27" t="s">
-        <v>340</v>
-      </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
@@ -7746,8 +7806,8 @@
       <c r="C63" t="s">
         <v>366</v>
       </c>
-      <c r="D63" s="4" t="s">
-        <v>323</v>
+      <c r="D63" s="22" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -7760,8 +7820,8 @@
       <c r="C64" t="s">
         <v>367</v>
       </c>
-      <c r="D64" t="s">
-        <v>404</v>
+      <c r="D64" s="22" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -7774,6 +7834,9 @@
       <c r="C65" t="s">
         <v>273</v>
       </c>
+      <c r="D65" s="22" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
@@ -7785,8 +7848,8 @@
       <c r="C66" t="s">
         <v>368</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>224</v>
+      <c r="D66" s="4" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -7799,8 +7862,8 @@
       <c r="C67" t="s">
         <v>337</v>
       </c>
-      <c r="D67" s="4" t="s">
-        <v>221</v>
+      <c r="D67" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -7813,9 +7876,6 @@
       <c r="C68" t="s">
         <v>309</v>
       </c>
-      <c r="D68" t="s">
-        <v>350</v>
-      </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
@@ -7827,16 +7887,16 @@
       <c r="C69" t="s">
         <v>306</v>
       </c>
-      <c r="D69" s="4" t="s">
-        <v>360</v>
+      <c r="D69" s="2" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="C70" t="s">
         <v>353</v>
       </c>
-      <c r="D70" s="19" t="s">
-        <v>228</v>
+      <c r="D70" s="4" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -7849,8 +7909,8 @@
       <c r="C71" t="s">
         <v>308</v>
       </c>
-      <c r="D71" s="4" t="s">
-        <v>304</v>
+      <c r="D71" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -7864,7 +7924,7 @@
         <v>352</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>222</v>
+        <v>360</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -7877,8 +7937,8 @@
       <c r="C73" t="s">
         <v>333</v>
       </c>
-      <c r="D73" s="4" t="s">
-        <v>248</v>
+      <c r="D73" s="19" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -7891,6 +7951,9 @@
       <c r="C74" s="19" t="s">
         <v>332</v>
       </c>
+      <c r="D74" s="4" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="8" t="s">
@@ -7902,6 +7965,9 @@
       <c r="C75" t="s">
         <v>380</v>
       </c>
+      <c r="D75" s="4" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
@@ -7909,6 +7975,9 @@
       </c>
       <c r="B76" t="s">
         <v>171</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="77" spans="1:4">

</xml_diff>

<commit_message>
Created comprehensive Android Pre-Launch To Do List based on issues identified in iOS Code Documentation. User info now added to Installation on app launch (as before), in addition to on log in/sign up (recent change). Created separate repo LinkMeUp-Analytics nested in Production and Analytics/EC2 Files (not included) to hold analytics suite. Added 5 Android (Galaxy S6) screenshots. Changed mobile number keypad to UIKeyboardTypeNumbersAndPunctuation to include return button, and updated/readded mobile number input sanitization code. Expanded -allVariantsOfContactNumber (Constants.m) to include phone number with +1 added to front. Changed -sanitizePhoneNumber: (Constants.m) to not strip phone numbers of plus signs, improving suggestions logic for int'l users. -sanitizePhoneNumber now called in -saveAddressBookContacts (Data.m). Removed special case code in contactsVC - links sent to self now appear in Recieved tab as well.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/LinkMeUp Planning Doc.xlsx
+++ b/Documents/Logs and Planning/LinkMeUp Planning Doc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6020" yWindow="3060" windowWidth="29620" windowHeight="20200" tabRatio="500"/>
+    <workbookView xWindow="41380" yWindow="0" windowWidth="22320" windowHeight="20200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="433">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -1059,12 +1059,6 @@
     <t>Settings/Privacy</t>
   </si>
   <si>
-    <t>Call to Action (IconShock) - $3</t>
-  </si>
-  <si>
-    <t>Launch Screen (IconShock) - $7</t>
-  </si>
-  <si>
     <t>Week 3</t>
   </si>
   <si>
@@ -1096,9 +1090,6 @@
   </si>
   <si>
     <t>Week 8</t>
-  </si>
-  <si>
-    <t>Prepare for launch</t>
   </si>
   <si>
     <t>Declare dictionary keys as constants</t>
@@ -1153,18 +1144,12 @@
     <t>Week 10</t>
   </si>
   <si>
-    <t>Twilio - $20</t>
-  </si>
-  <si>
     <t>Startup Career Fair - $46 (taxi) + $100 (fee)</t>
   </si>
   <si>
     <t xml:space="preserve">Atypical usernames absent from contactsVC </t>
   </si>
   <si>
-    <t>Remove trunk/Example and build/</t>
-  </si>
-  <si>
     <t>Remove unused frameworks</t>
   </si>
   <si>
@@ -1252,21 +1237,9 @@
     <t>Weebly Domain - $40 (x1)</t>
   </si>
   <si>
-    <t>App Icon (IconShock) - $20</t>
-  </si>
-  <si>
-    <t>Link sent to self should also go to Received tab</t>
-  </si>
-  <si>
     <t>Website</t>
   </si>
   <si>
-    <t>Change text message link to website URL</t>
-  </si>
-  <si>
-    <t>No "done" button in mobile verification keypad</t>
-  </si>
-  <si>
     <t>Week 11</t>
   </si>
   <si>
@@ -1324,18 +1297,9 @@
     <t>Switch to AWS Route 53 for DNS services</t>
   </si>
   <si>
-    <t>Get Android icon/launch screens produced</t>
-  </si>
-  <si>
-    <t>Look into alpha/beta testing procedures</t>
-  </si>
-  <si>
     <t>Test site on different browsers - IE, mobile</t>
   </si>
   <si>
-    <t>Get email list from ExactData</t>
-  </si>
-  <si>
     <t>Configure Google Analytics + FB Pixel</t>
   </si>
   <si>
@@ -1354,9 +1318,6 @@
     <t xml:space="preserve">Find source of current App Store traffic </t>
   </si>
   <si>
-    <t>Go through (recent) Android code</t>
-  </si>
-  <si>
     <t>Scrolling autocomplete results hides keyboard</t>
   </si>
   <si>
@@ -1387,9 +1348,6 @@
     <t>Friends VC search: bug w/ accepted request</t>
   </si>
   <si>
-    <t>Go through iOS code to determine min feature set</t>
-  </si>
-  <si>
     <t>Use Parse Analytics to track events/crashes</t>
   </si>
   <si>
@@ -1412,6 +1370,78 @@
   </si>
   <si>
     <t>Modularize local/server data update functions</t>
+  </si>
+  <si>
+    <t>Twilio - $20 (x2)</t>
+  </si>
+  <si>
+    <t>Remove trunk/Examples, build/, Echoprint Headers</t>
+  </si>
+  <si>
+    <t>Add README</t>
+  </si>
+  <si>
+    <t>v2.0 development</t>
+  </si>
+  <si>
+    <t>git; v2.0 development</t>
+  </si>
+  <si>
+    <t>promotional materials</t>
+  </si>
+  <si>
+    <t>press kit + emails</t>
+  </si>
+  <si>
+    <t>landing page + launch</t>
+  </si>
+  <si>
+    <t>Analytics + performance .py scripts; MongoDB course; documented iOS code; Android to do list</t>
+  </si>
+  <si>
+    <t>Website - Heyday code, resizing, footer links, refinement; signup flow docs; Thiel book</t>
+  </si>
+  <si>
+    <t>post-launch marketing; FB ads</t>
+  </si>
+  <si>
+    <t>server logging; new website</t>
+  </si>
+  <si>
+    <t>online contest; python</t>
+  </si>
+  <si>
+    <t>python; MongoDB; Android to do list</t>
+  </si>
+  <si>
+    <t>new website</t>
+  </si>
+  <si>
+    <t>Call to Action (Icon Shock) - $3</t>
+  </si>
+  <si>
+    <t>Launch Screen (Icon Shock) - $7</t>
+  </si>
+  <si>
+    <t>iOS App Icon (Ico nShock) - $20</t>
+  </si>
+  <si>
+    <t>Android Icon (Icon Shock) - $</t>
+  </si>
+  <si>
+    <t>Reintroduce 'link with Facebook' button</t>
+  </si>
+  <si>
+    <t>Broaden phone # match criteria in AB suggestions</t>
+  </si>
+  <si>
+    <t>Get Android icon produced</t>
+  </si>
+  <si>
+    <t>Test recent Android changes</t>
+  </si>
+  <si>
+    <t>Fill out Google Play Dev Console for beta release</t>
   </si>
 </sst>
 </file>
@@ -1592,8 +1622,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2519">
+  <cellStyleXfs count="2555">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4147,7 +4213,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2519">
+  <cellStyles count="2555">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5407,6 +5473,24 @@
     <cellStyle name="Followed Hyperlink" xfId="2514" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2516" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2520" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2524" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2526" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2528" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2530" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2532" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2534" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2536" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2538" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2540" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2542" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2544" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2550" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2554" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6666,6 +6750,24 @@
     <cellStyle name="Hyperlink" xfId="2513" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2515" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2519" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2523" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2525" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2527" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2529" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2531" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2533" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2535" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2537" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2539" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2541" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2543" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2549" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2553" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7000,8 +7102,8 @@
   </sheetPr>
   <dimension ref="A1:E178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7047,8 +7149,8 @@
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>373</v>
+      <c r="C4" s="27" t="s">
+        <v>429</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>298</v>
@@ -7063,15 +7165,15 @@
         <v>26</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>370</v>
+        <v>428</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="C6" s="27" t="s">
-        <v>372</v>
+      <c r="C6" s="22" t="s">
+        <v>393</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>118</v>
@@ -7084,8 +7186,8 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>406</v>
+      <c r="C7" s="23" t="s">
+        <v>391</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>299</v>
@@ -7098,8 +7200,8 @@
       <c r="B8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="23" t="s">
-        <v>404</v>
+      <c r="C8" s="22" t="s">
+        <v>394</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>284</v>
@@ -7113,7 +7215,7 @@
         <v>290</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -7126,8 +7228,8 @@
       <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>405</v>
+      <c r="C10" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -7137,11 +7239,11 @@
       <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
-        <v>408</v>
+      <c r="C11" s="4" t="s">
+        <v>287</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -7152,10 +7254,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>287</v>
+        <v>396</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -7166,16 +7268,16 @@
         <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="C14" s="4" t="s">
-        <v>410</v>
+      <c r="C14" t="s">
+        <v>398</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -7186,8 +7288,8 @@
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
-        <v>411</v>
+      <c r="C15" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>307</v>
@@ -7200,11 +7302,11 @@
       <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>129</v>
+      <c r="C16" s="18" t="s">
+        <v>190</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -7214,11 +7316,8 @@
       <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="18" t="s">
-        <v>190</v>
-      </c>
       <c r="D17" s="24" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -7252,10 +7351,10 @@
         <v>24</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -7266,7 +7365,7 @@
         <v>30</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="D21" s="22" t="s">
         <v>302</v>
@@ -7305,7 +7404,7 @@
         <v>33</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E24" s="11"/>
     </row>
@@ -7317,10 +7416,10 @@
         <v>53</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="E25" s="10"/>
     </row>
@@ -7335,7 +7434,7 @@
         <v>47</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -7349,7 +7448,7 @@
         <v>225</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -7374,7 +7473,7 @@
         <v>154</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -7382,7 +7481,7 @@
         <v>83</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -7396,7 +7495,7 @@
         <v>202</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -7410,7 +7509,7 @@
         <v>158</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -7430,7 +7529,7 @@
         <v>57</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>300</v>
@@ -7444,11 +7543,11 @@
       <c r="B35" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="27" t="s">
-        <v>396</v>
+      <c r="C35" s="22" t="s">
+        <v>388</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>414</v>
+        <v>430</v>
       </c>
       <c r="E35" s="12"/>
     </row>
@@ -7460,10 +7559,10 @@
         <v>59</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>400</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>393</v>
+        <v>386</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>431</v>
       </c>
       <c r="E36" s="18"/>
     </row>
@@ -7475,19 +7574,16 @@
         <v>60</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>398</v>
+        <v>357</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>403</v>
+        <v>432</v>
       </c>
       <c r="E37" s="10"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="C38" s="22" t="s">
-        <v>362</v>
-      </c>
-      <c r="D38" s="27" t="s">
-        <v>394</v>
+      <c r="C38" s="4" t="s">
+        <v>325</v>
       </c>
       <c r="E38" s="10"/>
     </row>
@@ -7499,10 +7595,7 @@
         <v>63</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="D39" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="E39" s="15"/>
     </row>
@@ -7513,9 +7606,6 @@
       <c r="B40" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>329</v>
-      </c>
       <c r="E40" s="16"/>
     </row>
     <row r="41" spans="1:5">
@@ -7535,10 +7625,10 @@
         <v>68</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="E42" s="9"/>
     </row>
@@ -7550,10 +7640,10 @@
         <v>72</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="E43" s="15"/>
     </row>
@@ -7565,10 +7655,10 @@
         <v>134</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -7579,19 +7669,19 @@
         <v>135</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="E45" s="15"/>
     </row>
     <row r="46" spans="1:5">
       <c r="C46" s="22" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="E46" s="15"/>
     </row>
@@ -7603,10 +7693,10 @@
         <v>75</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="E47" s="15"/>
     </row>
@@ -7618,10 +7708,10 @@
         <v>77</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -7632,7 +7722,7 @@
         <v>79</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -7643,10 +7733,10 @@
         <v>81</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -7657,7 +7747,7 @@
         <v>84</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="D51" s="27" t="s">
         <v>301</v>
@@ -7671,10 +7761,10 @@
         <v>100</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -7685,18 +7775,18 @@
         <v>92</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>339</v>
+        <v>410</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="C54" s="4" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -7707,7 +7797,10 @@
         <v>89</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>392</v>
+        <v>383</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -7729,7 +7822,7 @@
         <v>136</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -7743,7 +7836,7 @@
         <v>285</v>
       </c>
       <c r="D58" s="27" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -7757,7 +7850,7 @@
         <v>137</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -7768,10 +7861,10 @@
         <v>105</v>
       </c>
       <c r="C60" t="s">
-        <v>369</v>
+        <v>426</v>
       </c>
       <c r="D60" s="27" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -7782,18 +7875,18 @@
         <v>107</v>
       </c>
       <c r="C61" t="s">
-        <v>354</v>
-      </c>
-      <c r="D61" s="22" t="s">
-        <v>351</v>
+        <v>349</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="C62" t="s">
-        <v>336</v>
+        <v>409</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>324</v>
+        <v>346</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -7804,10 +7897,10 @@
         <v>109</v>
       </c>
       <c r="C63" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -7818,10 +7911,10 @@
         <v>111</v>
       </c>
       <c r="C64" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>419</v>
+        <v>321</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -7835,7 +7928,7 @@
         <v>273</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -7846,10 +7939,10 @@
         <v>128</v>
       </c>
       <c r="C66" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -7860,10 +7953,10 @@
         <v>116</v>
       </c>
       <c r="C67" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D67" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -7874,7 +7967,7 @@
         <v>121</v>
       </c>
       <c r="C68" t="s">
-        <v>309</v>
+        <v>425</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -7893,7 +7986,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="C70" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>221</v>
@@ -7907,10 +8000,10 @@
         <v>131</v>
       </c>
       <c r="C71" t="s">
-        <v>308</v>
+        <v>424</v>
       </c>
       <c r="D71" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -7921,10 +8014,10 @@
         <v>126</v>
       </c>
       <c r="C72" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -7935,7 +8028,7 @@
         <v>143</v>
       </c>
       <c r="C73" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D73" s="19" t="s">
         <v>228</v>
@@ -7949,7 +8042,7 @@
         <v>133</v>
       </c>
       <c r="C74" s="19" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>304</v>
@@ -7963,7 +8056,7 @@
         <v>132</v>
       </c>
       <c r="C75" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>222</v>
@@ -7976,6 +8069,9 @@
       <c r="B76" t="s">
         <v>171</v>
       </c>
+      <c r="C76" t="s">
+        <v>427</v>
+      </c>
       <c r="D76" s="4" t="s">
         <v>248</v>
       </c>
@@ -7987,13 +8083,10 @@
       <c r="B77" t="s">
         <v>172</v>
       </c>
-      <c r="C77" t="s">
-        <v>270</v>
-      </c>
     </row>
     <row r="78" spans="1:4">
       <c r="C78" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -8004,7 +8097,7 @@
         <v>141</v>
       </c>
       <c r="C79" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -8014,6 +8107,9 @@
       <c r="B80" t="s">
         <v>144</v>
       </c>
+      <c r="C80" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
@@ -8022,9 +8118,6 @@
       <c r="B81" t="s">
         <v>148</v>
       </c>
-      <c r="C81" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
@@ -8034,7 +8127,7 @@
         <v>147</v>
       </c>
       <c r="C82" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -8044,8 +8137,8 @@
       <c r="B83" t="s">
         <v>153</v>
       </c>
-      <c r="C83" s="25" t="s">
-        <v>330</v>
+      <c r="C83" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -8055,6 +8148,9 @@
       <c r="B84" t="s">
         <v>151</v>
       </c>
+      <c r="C84" s="25" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="13" t="s">
@@ -8221,7 +8317,7 @@
         <v>197</v>
       </c>
       <c r="B108" s="28" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -8515,7 +8611,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:3">
       <c r="A161" t="s">
         <v>282</v>
       </c>
@@ -8523,7 +8619,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:3">
       <c r="A163" t="s">
         <v>293</v>
       </c>
@@ -8531,7 +8627,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:3">
       <c r="A164" t="s">
         <v>296</v>
       </c>
@@ -8539,99 +8635,141 @@
         <v>295</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:3">
       <c r="A166" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:3">
       <c r="A167" t="s">
         <v>7</v>
       </c>
       <c r="B167" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2">
+        <v>366</v>
+      </c>
+      <c r="C167" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
       <c r="A168" t="s">
         <v>6</v>
       </c>
       <c r="B168" t="s">
+        <v>315</v>
+      </c>
+      <c r="C168" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" t="s">
+        <v>308</v>
+      </c>
+      <c r="B169" t="s">
+        <v>312</v>
+      </c>
+      <c r="C169" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" t="s">
+        <v>309</v>
+      </c>
+      <c r="B170" t="s">
+        <v>313</v>
+      </c>
+      <c r="C170" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" t="s">
+        <v>310</v>
+      </c>
+      <c r="B171" t="s">
+        <v>314</v>
+      </c>
+      <c r="C171" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" t="s">
+        <v>311</v>
+      </c>
+      <c r="B172" t="s">
+        <v>316</v>
+      </c>
+      <c r="C172" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="169" spans="1:2">
-      <c r="A169" t="s">
-        <v>310</v>
-      </c>
-      <c r="B169" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2">
-      <c r="A170" t="s">
-        <v>311</v>
-      </c>
-      <c r="B170" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2">
-      <c r="A171" t="s">
-        <v>312</v>
-      </c>
-      <c r="B171" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2">
-      <c r="A172" t="s">
-        <v>313</v>
-      </c>
-      <c r="B172" t="s">
+      <c r="B173" t="s">
+        <v>367</v>
+      </c>
+      <c r="C173" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="173" spans="1:2">
-      <c r="A173" t="s">
-        <v>319</v>
-      </c>
-      <c r="B173" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2">
-      <c r="A174" t="s">
-        <v>320</v>
-      </c>
       <c r="B174" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2">
+        <v>368</v>
+      </c>
+      <c r="C174" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B175" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2">
+        <v>369</v>
+      </c>
+      <c r="C175" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B176" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1">
+        <v>389</v>
+      </c>
+      <c r="C176" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1">
+        <v>365</v>
+      </c>
+      <c r="B177" t="s">
+        <v>418</v>
+      </c>
+      <c r="C177" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>379</v>
+        <v>370</v>
+      </c>
+      <c r="B178" t="s">
+        <v>417</v>
+      </c>
+      <c r="C178" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Android app icon files and feature graphic. Removed .pyc files from repo and added exclusion rule to .gitignore.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/LinkMeUp Planning Doc.xlsx
+++ b/Documents/Logs and Planning/LinkMeUp Planning Doc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="41380" yWindow="0" windowWidth="22320" windowHeight="20200" tabRatio="500"/>
+    <workbookView xWindow="41200" yWindow="2400" windowWidth="23000" windowHeight="12500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="434">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -1261,9 +1261,6 @@
     <t>Google Play Registration Fee - $25</t>
   </si>
   <si>
-    <t>Center App Store / Google Play Store badges</t>
-  </si>
-  <si>
     <t>Add icon to website logo</t>
   </si>
   <si>
@@ -1426,9 +1423,6 @@
     <t>iOS App Icon (Ico nShock) - $20</t>
   </si>
   <si>
-    <t>Android Icon (Icon Shock) - $</t>
-  </si>
-  <si>
     <t>Reintroduce 'link with Facebook' button</t>
   </si>
   <si>
@@ -1442,6 +1436,15 @@
   </si>
   <si>
     <t>Fill out Google Play Dev Console for beta release</t>
+  </si>
+  <si>
+    <t>Android Icon (Icon Shock) - $15</t>
+  </si>
+  <si>
+    <t>Replacing Coming Soon badge with Get It badge</t>
+  </si>
+  <si>
+    <t>Get SSL certificate for site (self-signed?)</t>
   </si>
 </sst>
 </file>
@@ -1622,8 +1625,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2555">
+  <cellStyleXfs count="2561">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4213,7 +4222,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2555">
+  <cellStyles count="2561">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5491,6 +5500,9 @@
     <cellStyle name="Followed Hyperlink" xfId="2550" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2552" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2560" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6768,6 +6780,9 @@
     <cellStyle name="Hyperlink" xfId="2549" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2551" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2559" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7102,8 +7117,8 @@
   </sheetPr>
   <dimension ref="A1:E178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="B41" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7150,7 +7165,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>298</v>
@@ -7165,7 +7180,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>340</v>
@@ -7173,7 +7188,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="C6" s="22" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>118</v>
@@ -7187,7 +7202,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>299</v>
@@ -7201,7 +7216,7 @@
         <v>43</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>284</v>
@@ -7215,7 +7230,7 @@
         <v>290</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -7229,7 +7244,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -7254,7 +7269,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>342</v>
@@ -7268,7 +7283,7 @@
         <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>339</v>
@@ -7277,7 +7292,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="C14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -7354,7 +7369,7 @@
         <v>359</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -7416,7 +7431,7 @@
         <v>53</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>351</v>
@@ -7473,7 +7488,7 @@
         <v>154</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -7481,7 +7496,7 @@
         <v>83</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -7509,7 +7524,7 @@
         <v>158</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -7544,10 +7559,10 @@
         <v>58</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E35" s="12"/>
     </row>
@@ -7559,10 +7574,10 @@
         <v>59</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E36" s="18"/>
     </row>
@@ -7577,7 +7592,7 @@
         <v>357</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E37" s="10"/>
     </row>
@@ -7639,11 +7654,11 @@
       <c r="B43" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C43" s="20" t="s">
-        <v>372</v>
+      <c r="C43" s="27" t="s">
+        <v>432</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E43" s="15"/>
     </row>
@@ -7655,10 +7670,10 @@
         <v>134</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -7669,7 +7684,7 @@
         <v>135</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D45" s="27" t="s">
         <v>358</v>
@@ -7678,10 +7693,10 @@
     </row>
     <row r="46" spans="1:5">
       <c r="C46" s="22" t="s">
-        <v>374</v>
+        <v>433</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E46" s="15"/>
     </row>
@@ -7693,10 +7708,10 @@
         <v>75</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E47" s="15"/>
     </row>
@@ -7708,7 +7723,7 @@
         <v>77</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D48" s="22" t="s">
         <v>337</v>
@@ -7722,7 +7737,7 @@
         <v>79</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -7733,7 +7748,7 @@
         <v>81</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>323</v>
@@ -7747,7 +7762,7 @@
         <v>84</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="D51" s="27" t="s">
         <v>301</v>
@@ -7760,8 +7775,8 @@
       <c r="B52" t="s">
         <v>100</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>380</v>
+      <c r="C52" s="22" t="s">
+        <v>376</v>
       </c>
       <c r="D52" s="27" t="s">
         <v>343</v>
@@ -7775,15 +7790,15 @@
         <v>92</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="C54" s="4" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D54" s="27" t="s">
         <v>335</v>
@@ -7797,10 +7812,10 @@
         <v>89</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -7810,6 +7825,9 @@
       <c r="B56" t="s">
         <v>90</v>
       </c>
+      <c r="C56" s="4" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
@@ -7818,12 +7836,6 @@
       <c r="B57" t="s">
         <v>97</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>344</v>
-      </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
@@ -7832,11 +7844,11 @@
       <c r="B58" t="s">
         <v>99</v>
       </c>
-      <c r="C58" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="D58" s="27" t="s">
-        <v>319</v>
+      <c r="C58" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -7847,10 +7859,10 @@
         <v>103</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>137</v>
+        <v>285</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -7860,11 +7872,11 @@
       <c r="B60" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C60" t="s">
-        <v>426</v>
+      <c r="C60" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="D60" s="27" t="s">
-        <v>354</v>
+        <v>322</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -7875,18 +7887,18 @@
         <v>107</v>
       </c>
       <c r="C61" t="s">
-        <v>349</v>
+        <v>425</v>
       </c>
       <c r="D61" s="27" t="s">
-        <v>405</v>
+        <v>354</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="C62" t="s">
-        <v>409</v>
-      </c>
-      <c r="D62" s="22" t="s">
-        <v>346</v>
+        <v>349</v>
+      </c>
+      <c r="D62" s="27" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -7897,10 +7909,10 @@
         <v>109</v>
       </c>
       <c r="C63" t="s">
-        <v>361</v>
+        <v>408</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>406</v>
+        <v>346</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -7911,10 +7923,10 @@
         <v>111</v>
       </c>
       <c r="C64" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>321</v>
+        <v>405</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -7925,10 +7937,10 @@
         <v>114</v>
       </c>
       <c r="C65" t="s">
-        <v>273</v>
+        <v>362</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>407</v>
+        <v>321</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -7939,10 +7951,10 @@
         <v>128</v>
       </c>
       <c r="C66" t="s">
-        <v>363</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>320</v>
+        <v>273</v>
+      </c>
+      <c r="D66" s="22" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -7953,10 +7965,10 @@
         <v>116</v>
       </c>
       <c r="C67" t="s">
-        <v>333</v>
-      </c>
-      <c r="D67" t="s">
-        <v>408</v>
+        <v>363</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -7967,7 +7979,10 @@
         <v>121</v>
       </c>
       <c r="C68" t="s">
-        <v>425</v>
+        <v>333</v>
+      </c>
+      <c r="D68" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -7978,18 +7993,15 @@
         <v>120</v>
       </c>
       <c r="C69" t="s">
-        <v>306</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>224</v>
+        <v>424</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="C70" t="s">
-        <v>348</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>221</v>
+        <v>306</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -8000,10 +8012,10 @@
         <v>131</v>
       </c>
       <c r="C71" t="s">
-        <v>424</v>
-      </c>
-      <c r="D71" t="s">
-        <v>345</v>
+        <v>348</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -8014,10 +8026,10 @@
         <v>126</v>
       </c>
       <c r="C72" t="s">
-        <v>347</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>355</v>
+        <v>423</v>
+      </c>
+      <c r="D72" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -8028,10 +8040,10 @@
         <v>143</v>
       </c>
       <c r="C73" t="s">
-        <v>330</v>
-      </c>
-      <c r="D73" s="19" t="s">
-        <v>228</v>
+        <v>347</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -8041,11 +8053,11 @@
       <c r="B74" t="s">
         <v>133</v>
       </c>
-      <c r="C74" s="19" t="s">
-        <v>329</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>304</v>
+      <c r="C74" t="s">
+        <v>330</v>
+      </c>
+      <c r="D74" s="19" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -8055,11 +8067,11 @@
       <c r="B75" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C75" t="s">
-        <v>371</v>
+      <c r="C75" s="19" t="s">
+        <v>329</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>222</v>
+        <v>304</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -8070,10 +8082,10 @@
         <v>171</v>
       </c>
       <c r="C76" t="s">
-        <v>427</v>
+        <v>371</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -8083,10 +8095,11 @@
       <c r="B77" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="C78" t="s">
-        <v>270</v>
+      <c r="C77" t="s">
+        <v>431</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -8097,7 +8110,7 @@
         <v>141</v>
       </c>
       <c r="C79" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -8108,7 +8121,7 @@
         <v>144</v>
       </c>
       <c r="C80" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -8118,6 +8131,9 @@
       <c r="B81" t="s">
         <v>148</v>
       </c>
+      <c r="C81" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
@@ -8126,9 +8142,6 @@
       <c r="B82" t="s">
         <v>147</v>
       </c>
-      <c r="C82" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
@@ -8138,7 +8151,7 @@
         <v>153</v>
       </c>
       <c r="C83" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -8148,8 +8161,8 @@
       <c r="B84" t="s">
         <v>151</v>
       </c>
-      <c r="C84" s="25" t="s">
-        <v>327</v>
+      <c r="C84" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -8159,6 +8172,9 @@
       <c r="B85" s="13" t="s">
         <v>155</v>
       </c>
+      <c r="C85" s="25" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
@@ -8648,7 +8664,7 @@
         <v>366</v>
       </c>
       <c r="C167" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -8659,7 +8675,7 @@
         <v>315</v>
       </c>
       <c r="C168" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -8670,7 +8686,7 @@
         <v>312</v>
       </c>
       <c r="C169" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -8681,7 +8697,7 @@
         <v>313</v>
       </c>
       <c r="C170" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -8692,7 +8708,7 @@
         <v>314</v>
       </c>
       <c r="C171" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -8703,7 +8719,7 @@
         <v>316</v>
       </c>
       <c r="C172" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -8714,7 +8730,7 @@
         <v>367</v>
       </c>
       <c r="C173" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -8725,7 +8741,7 @@
         <v>368</v>
       </c>
       <c r="C174" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -8736,7 +8752,7 @@
         <v>369</v>
       </c>
       <c r="C175" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -8744,10 +8760,10 @@
         <v>332</v>
       </c>
       <c r="B176" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C176" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -8755,10 +8771,10 @@
         <v>365</v>
       </c>
       <c r="B177" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C177" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -8766,10 +8782,10 @@
         <v>370</v>
       </c>
       <c r="B178" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C178" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revised contest_drawing.py logic to include users with Western WA phone numbers beginning with "+1" in contest. Added new contest image and Facebook cover photo (with Google Play badge).
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/LinkMeUp Planning Doc.xlsx
+++ b/Documents/Logs and Planning/LinkMeUp Planning Doc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="41200" yWindow="2400" windowWidth="23000" windowHeight="12500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30000" windowHeight="23260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="436">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -1074,13 +1074,7 @@
     <t>Scrollable button label; push notif/AB permissions flow; interv. Calvin; posted to FB groups</t>
   </si>
   <si>
-    <t>Changed searchVC UI; new launch screens; general debugging/testing; interv. Sean</t>
-  </si>
-  <si>
     <t>Master links; screenshots; offer/contract for Sean; submitted archive; created app video</t>
-  </si>
-  <si>
-    <t>ContactsVC - sending texts to non-users, Recents section, icons and UI; LinkedIn inMail</t>
   </si>
   <si>
     <t>Finalized video; helped Sean; created press kit; emails to 19 journalists (+7 review sites)</t>
@@ -1135,9 +1129,6 @@
     <t>Facebook Ads - $119.61</t>
   </si>
   <si>
-    <t>Android Development - $2250</t>
-  </si>
-  <si>
     <t>Week 9</t>
   </si>
   <si>
@@ -1186,12 +1177,6 @@
     <t>Replace setObj, objForKey, initWithObjs w/literals</t>
   </si>
   <si>
-    <t>Vimeo Video Hosting - $10 (x1)</t>
-  </si>
-  <si>
-    <t>Google Apps - $5 (x1)</t>
-  </si>
-  <si>
     <t>iPhone 5 Restocking Fee - $35 (x2)</t>
   </si>
   <si>
@@ -1303,18 +1288,12 @@
     <t>Buy appshout! Noise package</t>
   </si>
   <si>
-    <t>Write analytics suite to analyze existing data</t>
-  </si>
-  <si>
     <t>Promote contest (FB ads, etc)</t>
   </si>
   <si>
     <t>Server logging; FB signup issue; new website - AWS S3, Endless' code, embedding video</t>
   </si>
   <si>
-    <t xml:space="preserve">Find source of current App Store traffic </t>
-  </si>
-  <si>
     <t>Scrolling autocomplete results hides keyboard</t>
   </si>
   <si>
@@ -1354,9 +1333,6 @@
     <t>Renew/replace push certificates</t>
   </si>
   <si>
-    <t>Support iOS 9/Xcode 7</t>
-  </si>
-  <si>
     <t>Replace for loops with for each loops</t>
   </si>
   <si>
@@ -1378,21 +1354,6 @@
     <t>Add README</t>
   </si>
   <si>
-    <t>v2.0 development</t>
-  </si>
-  <si>
-    <t>git; v2.0 development</t>
-  </si>
-  <si>
-    <t>promotional materials</t>
-  </si>
-  <si>
-    <t>press kit + emails</t>
-  </si>
-  <si>
-    <t>landing page + launch</t>
-  </si>
-  <si>
     <t>Analytics + performance .py scripts; MongoDB course; documented iOS code; Android to do list</t>
   </si>
   <si>
@@ -1420,31 +1381,76 @@
     <t>Launch Screen (Icon Shock) - $7</t>
   </si>
   <si>
-    <t>iOS App Icon (Ico nShock) - $20</t>
-  </si>
-  <si>
     <t>Reintroduce 'link with Facebook' button</t>
   </si>
   <si>
     <t>Broaden phone # match criteria in AB suggestions</t>
   </si>
   <si>
-    <t>Get Android icon produced</t>
-  </si>
-  <si>
-    <t>Test recent Android changes</t>
-  </si>
-  <si>
-    <t>Fill out Google Play Dev Console for beta release</t>
-  </si>
-  <si>
     <t>Android Icon (Icon Shock) - $15</t>
   </si>
   <si>
-    <t>Replacing Coming Soon badge with Get It badge</t>
-  </si>
-  <si>
     <t>Get SSL certificate for site (self-signed?)</t>
+  </si>
+  <si>
+    <t>Replace Coming Soon to GP w/ Get It On GP badge</t>
+  </si>
+  <si>
+    <t>Do round 2 of beta testing (esp. w/ int'l users)</t>
+  </si>
+  <si>
+    <t>Prepare for public launch on 9/5</t>
+  </si>
+  <si>
+    <t>Week 13</t>
+  </si>
+  <si>
+    <t>Week 14</t>
+  </si>
+  <si>
+    <t>Vimeo Video Hosting - $10 (x3)</t>
+  </si>
+  <si>
+    <t>Android Development - $5712.50</t>
+  </si>
+  <si>
+    <t>iOS App Icon (Icon Shock) - $20</t>
+  </si>
+  <si>
+    <t>Support iOS 9 (Xcode 7)</t>
+  </si>
+  <si>
+    <t>landing page; public launch</t>
+  </si>
+  <si>
+    <t>video; press kit; emails</t>
+  </si>
+  <si>
+    <t>git; AB integration</t>
+  </si>
+  <si>
+    <t>permissions flow</t>
+  </si>
+  <si>
+    <t>SMS links; contactsVC; InMail</t>
+  </si>
+  <si>
+    <t>ContactsVC - sending texts to non-users, Recents section, icons and UI; LinkedIn InMail</t>
+  </si>
+  <si>
+    <t>searchVC; launch screen; testing</t>
+  </si>
+  <si>
+    <t>Changed searchVC UI; new launch screens; interv. Sean; general debugging/testing</t>
+  </si>
+  <si>
+    <t>master links; screenshots; app video</t>
+  </si>
+  <si>
+    <t>Ssend survey email to users about app discovery</t>
+  </si>
+  <si>
+    <t>Google Apps - $5 (x2)</t>
   </si>
 </sst>
 </file>
@@ -1625,8 +1631,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2561">
+  <cellStyleXfs count="2573">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4222,7 +4240,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2561">
+  <cellStyles count="2573">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5503,6 +5521,12 @@
     <cellStyle name="Followed Hyperlink" xfId="2556" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2558" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2564" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2572" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6783,6 +6807,12 @@
     <cellStyle name="Hyperlink" xfId="2555" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2557" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2563" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2571" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7115,10 +7145,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E178"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7165,7 +7195,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>298</v>
@@ -7180,15 +7210,15 @@
         <v>26</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="C6" s="22" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>118</v>
@@ -7202,7 +7232,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>299</v>
@@ -7216,7 +7246,7 @@
         <v>43</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>284</v>
@@ -7230,7 +7260,7 @@
         <v>290</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -7244,7 +7274,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -7258,7 +7288,7 @@
         <v>287</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -7269,10 +7299,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -7283,16 +7313,16 @@
         <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
       <c r="C14" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -7321,7 +7351,7 @@
         <v>190</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -7332,7 +7362,7 @@
         <v>29</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -7366,10 +7396,10 @@
         <v>24</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -7380,7 +7410,7 @@
         <v>30</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D21" s="22" t="s">
         <v>302</v>
@@ -7419,7 +7449,7 @@
         <v>33</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E24" s="11"/>
     </row>
@@ -7431,10 +7461,10 @@
         <v>53</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="E25" s="10"/>
     </row>
@@ -7448,8 +7478,8 @@
       <c r="C26" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>352</v>
+      <c r="D26" s="27" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -7463,7 +7493,7 @@
         <v>225</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -7488,15 +7518,15 @@
         <v>154</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="C30" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D30" s="27" t="s">
-        <v>402</v>
+      <c r="D30" s="20" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -7510,7 +7540,7 @@
         <v>202</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -7524,7 +7554,7 @@
         <v>158</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>403</v>
+        <v>424</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -7544,7 +7574,7 @@
         <v>57</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>300</v>
@@ -7558,11 +7588,11 @@
       <c r="B35" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="22" t="s">
-        <v>387</v>
+      <c r="C35" s="27" t="s">
+        <v>381</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E35" s="12"/>
     </row>
@@ -7574,10 +7604,10 @@
         <v>59</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>385</v>
-      </c>
-      <c r="D36" s="27" t="s">
-        <v>429</v>
+        <v>380</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>418</v>
       </c>
       <c r="E36" s="18"/>
     </row>
@@ -7589,16 +7619,13 @@
         <v>60</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>357</v>
-      </c>
-      <c r="D37" s="27" t="s">
-        <v>430</v>
+        <v>352</v>
       </c>
       <c r="E37" s="10"/>
     </row>
     <row r="38" spans="1:5">
       <c r="C38" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E38" s="10"/>
     </row>
@@ -7610,7 +7637,7 @@
         <v>63</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E39" s="15"/>
     </row>
@@ -7640,10 +7667,10 @@
         <v>68</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E42" s="9"/>
     </row>
@@ -7655,10 +7682,10 @@
         <v>72</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>389</v>
+        <v>434</v>
       </c>
       <c r="E43" s="15"/>
     </row>
@@ -7670,10 +7697,10 @@
         <v>134</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>372</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>386</v>
+        <v>367</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -7684,19 +7711,19 @@
         <v>135</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>358</v>
+        <v>379</v>
       </c>
       <c r="E45" s="15"/>
     </row>
     <row r="46" spans="1:5">
       <c r="C46" s="22" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="E46" s="15"/>
     </row>
@@ -7708,10 +7735,10 @@
         <v>75</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>373</v>
-      </c>
-      <c r="D47" s="27" t="s">
-        <v>400</v>
+        <v>368</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>334</v>
       </c>
       <c r="E47" s="15"/>
     </row>
@@ -7723,10 +7750,7 @@
         <v>77</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>374</v>
-      </c>
-      <c r="D48" s="22" t="s">
-        <v>337</v>
+        <v>369</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -7737,7 +7761,7 @@
         <v>79</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -7748,10 +7772,10 @@
         <v>81</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -7762,7 +7786,7 @@
         <v>84</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="D51" s="27" t="s">
         <v>301</v>
@@ -7776,10 +7800,10 @@
         <v>100</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -7790,18 +7814,18 @@
         <v>92</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="C54" s="4" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -7812,10 +7836,10 @@
         <v>89</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -7826,7 +7850,7 @@
         <v>90</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -7848,7 +7872,7 @@
         <v>136</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -7862,7 +7886,7 @@
         <v>285</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -7876,7 +7900,7 @@
         <v>137</v>
       </c>
       <c r="D60" s="27" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -7887,18 +7911,18 @@
         <v>107</v>
       </c>
       <c r="C61" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D61" s="27" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="C62" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D62" s="27" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -7909,10 +7933,10 @@
         <v>109</v>
       </c>
       <c r="C63" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -7923,10 +7947,10 @@
         <v>111</v>
       </c>
       <c r="C64" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -7937,10 +7961,10 @@
         <v>114</v>
       </c>
       <c r="C65" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -7954,7 +7978,7 @@
         <v>273</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -7965,10 +7989,10 @@
         <v>116</v>
       </c>
       <c r="C67" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -7979,10 +8003,10 @@
         <v>121</v>
       </c>
       <c r="C68" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D68" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -7993,7 +8017,7 @@
         <v>120</v>
       </c>
       <c r="C69" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -8012,7 +8036,7 @@
         <v>131</v>
       </c>
       <c r="C71" t="s">
-        <v>348</v>
+        <v>435</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>221</v>
@@ -8026,10 +8050,10 @@
         <v>126</v>
       </c>
       <c r="C72" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="D72" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -8040,10 +8064,10 @@
         <v>143</v>
       </c>
       <c r="C73" t="s">
-        <v>347</v>
+        <v>421</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -8054,7 +8078,7 @@
         <v>133</v>
       </c>
       <c r="C74" t="s">
-        <v>330</v>
+        <v>422</v>
       </c>
       <c r="D74" s="19" t="s">
         <v>228</v>
@@ -8068,7 +8092,7 @@
         <v>132</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>304</v>
@@ -8082,7 +8106,7 @@
         <v>171</v>
       </c>
       <c r="C76" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>222</v>
@@ -8096,7 +8120,7 @@
         <v>172</v>
       </c>
       <c r="C77" t="s">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>248</v>
@@ -8173,7 +8197,7 @@
         <v>155</v>
       </c>
       <c r="C85" s="25" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -8333,7 +8357,7 @@
         <v>197</v>
       </c>
       <c r="B108" s="28" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -8661,10 +8685,10 @@
         <v>7</v>
       </c>
       <c r="B167" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C167" t="s">
-        <v>412</v>
+        <v>427</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -8672,10 +8696,10 @@
         <v>6</v>
       </c>
       <c r="B168" t="s">
-        <v>315</v>
+        <v>430</v>
       </c>
       <c r="C168" t="s">
-        <v>411</v>
+        <v>429</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -8686,7 +8710,7 @@
         <v>312</v>
       </c>
       <c r="C169" t="s">
-        <v>411</v>
+        <v>428</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -8694,10 +8718,10 @@
         <v>309</v>
       </c>
       <c r="B170" t="s">
-        <v>313</v>
+        <v>432</v>
       </c>
       <c r="C170" t="s">
-        <v>411</v>
+        <v>431</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -8705,10 +8729,10 @@
         <v>310</v>
       </c>
       <c r="B171" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C171" t="s">
-        <v>413</v>
+        <v>433</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -8716,82 +8740,91 @@
         <v>311</v>
       </c>
       <c r="B172" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C172" t="s">
-        <v>414</v>
+        <v>426</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B173" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C173" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B174" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C174" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B175" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="C175" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B176" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="C176" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="B177" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
       <c r="C177" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B178" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="C178" t="s">
-        <v>421</v>
+        <v>408</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" t="s">
+        <v>420</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
No major changes (besides update to Planning Doc) - commit made to isolate subsequent folder reorganization/deletions.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/LinkMeUp Planning Doc.xlsx
+++ b/Documents/Logs and Planning/LinkMeUp Planning Doc.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="437">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -1035,9 +1035,6 @@
     <t>Favorite links</t>
   </si>
   <si>
-    <t>Android Development</t>
-  </si>
-  <si>
     <t>Test LMU app build on another computer</t>
   </si>
   <si>
@@ -1288,9 +1285,6 @@
     <t>Buy appshout! Noise package</t>
   </si>
   <si>
-    <t>Promote contest (FB ads, etc)</t>
-  </si>
-  <si>
     <t>Server logging; FB signup issue; new website - AWS S3, Endless' code, embedding video</t>
   </si>
   <si>
@@ -1399,9 +1393,6 @@
     <t>Do round 2 of beta testing (esp. w/ int'l users)</t>
   </si>
   <si>
-    <t>Prepare for public launch on 9/5</t>
-  </si>
-  <si>
     <t>Week 13</t>
   </si>
   <si>
@@ -1447,10 +1438,22 @@
     <t>master links; screenshots; app video</t>
   </si>
   <si>
-    <t>Ssend survey email to users about app discovery</t>
-  </si>
-  <si>
     <t>Google Apps - $5 (x2)</t>
+  </si>
+  <si>
+    <t>Send survey email to users about app discovery</t>
+  </si>
+  <si>
+    <t>Prepare for public launch on 9/6</t>
+  </si>
+  <si>
+    <t>Android Development/Launch</t>
+  </si>
+  <si>
+    <t>Ask active users (&gt;1 link sent) to rate/review app</t>
+  </si>
+  <si>
+    <t>Add referral incentive + restart online contest</t>
   </si>
 </sst>
 </file>
@@ -1590,7 +1593,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1621,6 +1624,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1631,7 +1640,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2573">
+  <cellStyleXfs count="2577">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4205,8 +4214,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4239,8 +4252,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2573">
+  <cellStyles count="2577">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5527,6 +5541,8 @@
     <cellStyle name="Followed Hyperlink" xfId="2568" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2570" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2576" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6813,6 +6829,8 @@
     <cellStyle name="Hyperlink" xfId="2567" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2569" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2575" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7147,8 +7165,8 @@
   </sheetPr>
   <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7195,7 +7213,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>298</v>
@@ -7210,15 +7228,15 @@
         <v>26</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="C6" s="22" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>118</v>
@@ -7232,7 +7250,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>299</v>
@@ -7246,7 +7264,7 @@
         <v>43</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>284</v>
@@ -7260,7 +7278,7 @@
         <v>290</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -7274,7 +7292,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -7288,7 +7306,7 @@
         <v>287</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -7299,10 +7317,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -7313,16 +7331,16 @@
         <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
       <c r="C14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -7337,7 +7355,7 @@
         <v>129</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -7351,7 +7369,7 @@
         <v>190</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -7362,7 +7380,7 @@
         <v>29</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -7396,10 +7414,10 @@
         <v>24</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -7410,10 +7428,10 @@
         <v>30</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E21" s="11"/>
     </row>
@@ -7422,7 +7440,7 @@
         <v>286</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E22" s="11"/>
     </row>
@@ -7437,7 +7455,7 @@
         <v>261</v>
       </c>
       <c r="D23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E23" s="9"/>
     </row>
@@ -7449,7 +7467,7 @@
         <v>33</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E24" s="11"/>
     </row>
@@ -7461,10 +7479,10 @@
         <v>53</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E25" s="10"/>
     </row>
@@ -7479,7 +7497,7 @@
         <v>47</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -7493,7 +7511,7 @@
         <v>225</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -7518,7 +7536,7 @@
         <v>154</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -7526,7 +7544,7 @@
         <v>83</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -7540,7 +7558,7 @@
         <v>202</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -7554,7 +7572,7 @@
         <v>158</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -7574,10 +7592,10 @@
         <v>57</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>300</v>
+        <v>434</v>
       </c>
       <c r="E34" s="10"/>
     </row>
@@ -7588,11 +7606,11 @@
       <c r="B35" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="27" t="s">
-        <v>381</v>
+      <c r="C35" s="20" t="s">
+        <v>435</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E35" s="12"/>
     </row>
@@ -7603,11 +7621,11 @@
       <c r="B36" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="22" t="s">
-        <v>380</v>
+      <c r="C36" s="32" t="s">
+        <v>436</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>418</v>
+        <v>433</v>
       </c>
       <c r="E36" s="18"/>
     </row>
@@ -7619,13 +7637,13 @@
         <v>60</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>352</v>
+        <v>379</v>
       </c>
       <c r="E37" s="10"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="C38" s="4" t="s">
-        <v>323</v>
+      <c r="C38" s="22" t="s">
+        <v>351</v>
       </c>
       <c r="E38" s="10"/>
     </row>
@@ -7637,7 +7655,7 @@
         <v>63</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E39" s="15"/>
     </row>
@@ -7648,6 +7666,9 @@
       <c r="B40" t="s">
         <v>67</v>
       </c>
+      <c r="C40" s="4" t="s">
+        <v>323</v>
+      </c>
       <c r="E40" s="16"/>
     </row>
     <row r="41" spans="1:5">
@@ -7667,10 +7688,10 @@
         <v>68</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E42" s="9"/>
     </row>
@@ -7681,11 +7702,11 @@
       <c r="B43" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C43" s="27" t="s">
-        <v>416</v>
+      <c r="C43" s="20" t="s">
+        <v>414</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E43" s="15"/>
     </row>
@@ -7697,10 +7718,10 @@
         <v>134</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -7711,19 +7732,19 @@
         <v>135</v>
       </c>
       <c r="C45" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="D45" s="27" t="s">
         <v>378</v>
-      </c>
-      <c r="D45" s="27" t="s">
-        <v>379</v>
       </c>
       <c r="E45" s="15"/>
     </row>
     <row r="46" spans="1:5">
       <c r="C46" s="22" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E46" s="15"/>
     </row>
@@ -7735,10 +7756,10 @@
         <v>75</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E47" s="15"/>
     </row>
@@ -7750,7 +7771,7 @@
         <v>77</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -7761,7 +7782,7 @@
         <v>79</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -7772,10 +7793,10 @@
         <v>81</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -7786,10 +7807,10 @@
         <v>84</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -7800,10 +7821,10 @@
         <v>100</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -7814,18 +7835,18 @@
         <v>92</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="C54" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -7836,10 +7857,10 @@
         <v>89</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -7850,7 +7871,7 @@
         <v>90</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -7872,7 +7893,7 @@
         <v>136</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -7886,7 +7907,7 @@
         <v>285</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -7900,7 +7921,7 @@
         <v>137</v>
       </c>
       <c r="D60" s="27" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -7911,18 +7932,18 @@
         <v>107</v>
       </c>
       <c r="C61" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D61" s="27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="C62" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D62" s="27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -7933,10 +7954,10 @@
         <v>109</v>
       </c>
       <c r="C63" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -7947,10 +7968,10 @@
         <v>111</v>
       </c>
       <c r="C64" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -7961,10 +7982,10 @@
         <v>114</v>
       </c>
       <c r="C65" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -7978,7 +7999,7 @@
         <v>273</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -7989,10 +8010,10 @@
         <v>116</v>
       </c>
       <c r="C67" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -8003,10 +8024,10 @@
         <v>121</v>
       </c>
       <c r="C68" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D68" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -8017,12 +8038,12 @@
         <v>120</v>
       </c>
       <c r="C69" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="C70" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>224</v>
@@ -8036,7 +8057,7 @@
         <v>131</v>
       </c>
       <c r="C71" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>221</v>
@@ -8050,10 +8071,10 @@
         <v>126</v>
       </c>
       <c r="C72" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D72" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -8064,10 +8085,10 @@
         <v>143</v>
       </c>
       <c r="C73" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -8078,7 +8099,7 @@
         <v>133</v>
       </c>
       <c r="C74" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D74" s="19" t="s">
         <v>228</v>
@@ -8092,10 +8113,10 @@
         <v>132</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -8106,7 +8127,7 @@
         <v>171</v>
       </c>
       <c r="C76" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>222</v>
@@ -8120,7 +8141,7 @@
         <v>172</v>
       </c>
       <c r="C77" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>248</v>
@@ -8197,7 +8218,7 @@
         <v>155</v>
       </c>
       <c r="C85" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -8357,7 +8378,7 @@
         <v>197</v>
       </c>
       <c r="B108" s="28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -8685,10 +8706,10 @@
         <v>7</v>
       </c>
       <c r="B167" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C167" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -8696,135 +8717,136 @@
         <v>6</v>
       </c>
       <c r="B168" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C168" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B169" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C169" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B170" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C170" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B171" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C171" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B172" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C172" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B173" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C173" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B174" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C174" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B175" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C175" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B176" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C176" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B177" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C177" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B178" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C178" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Created file "Contest 2 Materials" with contents of Facebook posts and text message to be sent on Android launch. Updated send_Twilio_SMS.py with new launch message.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/LinkMeUp Planning Doc.xlsx
+++ b/Documents/Logs and Planning/LinkMeUp Planning Doc.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="436">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -1244,9 +1244,6 @@
   </si>
   <si>
     <t>Add icon to website logo</t>
-  </si>
-  <si>
-    <t>Properly configure meta OG share image</t>
   </si>
   <si>
     <t>Add/optimize meta keywords</t>
@@ -1640,8 +1637,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2577">
+  <cellStyleXfs count="2579">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4254,7 +4253,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2577">
+  <cellStyles count="2579">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5543,6 +5542,7 @@
     <cellStyle name="Followed Hyperlink" xfId="2572" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2574" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2578" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6831,6 +6831,7 @@
     <cellStyle name="Hyperlink" xfId="2571" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2573" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2577" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7165,8 +7166,8 @@
   </sheetPr>
   <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7213,7 +7214,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>298</v>
@@ -7228,7 +7229,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>336</v>
@@ -7236,7 +7237,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="C6" s="22" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>118</v>
@@ -7250,7 +7251,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>299</v>
@@ -7264,7 +7265,7 @@
         <v>43</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>284</v>
@@ -7278,7 +7279,7 @@
         <v>290</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -7292,7 +7293,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -7317,7 +7318,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>338</v>
@@ -7331,7 +7332,7 @@
         <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>335</v>
@@ -7340,7 +7341,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="C14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -7417,7 +7418,7 @@
         <v>353</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -7479,7 +7480,7 @@
         <v>53</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>345</v>
@@ -7536,7 +7537,7 @@
         <v>154</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -7544,7 +7545,7 @@
         <v>83</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -7572,7 +7573,7 @@
         <v>158</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -7595,7 +7596,7 @@
         <v>334</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E34" s="10"/>
     </row>
@@ -7607,10 +7608,10 @@
         <v>58</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E35" s="12"/>
     </row>
@@ -7622,10 +7623,10 @@
         <v>59</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E36" s="18"/>
     </row>
@@ -7637,7 +7638,7 @@
         <v>60</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E37" s="10"/>
     </row>
@@ -7703,10 +7704,10 @@
         <v>72</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E43" s="15"/>
     </row>
@@ -7732,19 +7733,19 @@
         <v>135</v>
       </c>
       <c r="C45" s="27" t="s">
+        <v>376</v>
+      </c>
+      <c r="D45" s="27" t="s">
         <v>377</v>
-      </c>
-      <c r="D45" s="27" t="s">
-        <v>378</v>
       </c>
       <c r="E45" s="15"/>
     </row>
     <row r="46" spans="1:5">
       <c r="C46" s="22" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E46" s="15"/>
     </row>
@@ -7771,7 +7772,7 @@
         <v>77</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -7782,7 +7783,7 @@
         <v>79</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -7793,7 +7794,7 @@
         <v>81</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>320</v>
@@ -7807,7 +7808,7 @@
         <v>84</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D51" s="27" t="s">
         <v>300</v>
@@ -7820,8 +7821,8 @@
       <c r="B52" t="s">
         <v>100</v>
       </c>
-      <c r="C52" s="22" t="s">
-        <v>370</v>
+      <c r="C52" s="4" t="s">
+        <v>372</v>
       </c>
       <c r="D52" s="27" t="s">
         <v>339</v>
@@ -7835,15 +7836,15 @@
         <v>92</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="C54" s="4" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D54" s="27" t="s">
         <v>331</v>
@@ -7860,7 +7861,7 @@
         <v>375</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -7870,9 +7871,6 @@
       <c r="B56" t="s">
         <v>90</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>376</v>
-      </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
@@ -7932,7 +7930,7 @@
         <v>107</v>
       </c>
       <c r="C61" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D61" s="27" t="s">
         <v>348</v>
@@ -7943,7 +7941,7 @@
         <v>343</v>
       </c>
       <c r="D62" s="27" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -7954,7 +7952,7 @@
         <v>109</v>
       </c>
       <c r="C63" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D63" s="22" t="s">
         <v>342</v>
@@ -7971,7 +7969,7 @@
         <v>355</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -7999,7 +7997,7 @@
         <v>273</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -8027,7 +8025,7 @@
         <v>329</v>
       </c>
       <c r="D68" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -8038,7 +8036,7 @@
         <v>120</v>
       </c>
       <c r="C69" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -8057,7 +8055,7 @@
         <v>131</v>
       </c>
       <c r="C71" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>221</v>
@@ -8071,7 +8069,7 @@
         <v>126</v>
       </c>
       <c r="C72" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D72" t="s">
         <v>341</v>
@@ -8085,7 +8083,7 @@
         <v>143</v>
       </c>
       <c r="C73" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>349</v>
@@ -8099,7 +8097,7 @@
         <v>133</v>
       </c>
       <c r="C74" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D74" s="19" t="s">
         <v>228</v>
@@ -8141,7 +8139,7 @@
         <v>172</v>
       </c>
       <c r="C77" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>248</v>
@@ -8709,7 +8707,7 @@
         <v>360</v>
       </c>
       <c r="C167" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -8717,10 +8715,10 @@
         <v>6</v>
       </c>
       <c r="B168" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C168" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -8731,7 +8729,7 @@
         <v>311</v>
       </c>
       <c r="C169" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -8739,10 +8737,10 @@
         <v>308</v>
       </c>
       <c r="B170" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C170" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -8753,7 +8751,7 @@
         <v>312</v>
       </c>
       <c r="C171" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -8764,7 +8762,7 @@
         <v>313</v>
       </c>
       <c r="C172" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -8775,7 +8773,7 @@
         <v>361</v>
       </c>
       <c r="C173" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -8786,7 +8784,7 @@
         <v>362</v>
       </c>
       <c r="C174" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -8797,7 +8795,7 @@
         <v>363</v>
       </c>
       <c r="C175" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -8805,10 +8803,10 @@
         <v>328</v>
       </c>
       <c r="B176" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C176" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -8816,10 +8814,10 @@
         <v>359</v>
       </c>
       <c r="B177" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C177" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -8827,25 +8825,26 @@
         <v>364</v>
       </c>
       <c r="B178" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C178" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Modified get_mobile_numbers.py to only print out mobile numbers of old users (i.e. accounts not created in last 3 days). Changed/finalized content of text message sent on launch (Contest 2 Materials.docx, send_Twilio_SMS.py). Added file count_mobile_numbers.py.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/LinkMeUp Planning Doc.xlsx
+++ b/Documents/Logs and Planning/LinkMeUp Planning Doc.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="433">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -1035,9 +1035,6 @@
     <t>Favorite links</t>
   </si>
   <si>
-    <t>Test LMU app build on another computer</t>
-  </si>
-  <si>
     <t>Using file system cache to improve link load time</t>
   </si>
   <si>
@@ -1162,9 +1159,6 @@
     <t>Web page (news articles) links</t>
   </si>
   <si>
-    <t>Regroup and rename classes in project</t>
-  </si>
-  <si>
     <t>Coding Style / Conventions</t>
   </si>
   <si>
@@ -1189,9 +1183,6 @@
     <t>Consider alternative backend stacks</t>
   </si>
   <si>
-    <t>Replace IS_IPHONE5 with new IS_IPHONE_5</t>
-  </si>
-  <si>
     <t>Use of device/OS macros</t>
   </si>
   <si>
@@ -1321,9 +1312,6 @@
     <t>Updates</t>
   </si>
   <si>
-    <t>Renew/replace push certificates</t>
-  </si>
-  <si>
     <t>Replace for loops with for each loops</t>
   </si>
   <si>
@@ -1339,12 +1327,6 @@
     <t>Twilio - $20 (x2)</t>
   </si>
   <si>
-    <t>Remove trunk/Examples, build/, Echoprint Headers</t>
-  </si>
-  <si>
-    <t>Add README</t>
-  </si>
-  <si>
     <t>Analytics + performance .py scripts; MongoDB course; documented iOS code; Android to do list</t>
   </si>
   <si>
@@ -1384,12 +1366,6 @@
     <t>Get SSL certificate for site (self-signed?)</t>
   </si>
   <si>
-    <t>Replace Coming Soon to GP w/ Get It On GP badge</t>
-  </si>
-  <si>
-    <t>Do round 2 of beta testing (esp. w/ int'l users)</t>
-  </si>
-  <si>
     <t>Week 13</t>
   </si>
   <si>
@@ -1441,23 +1417,38 @@
     <t>Send survey email to users about app discovery</t>
   </si>
   <si>
-    <t>Prepare for public launch on 9/6</t>
-  </si>
-  <si>
     <t>Android Development/Launch</t>
   </si>
   <si>
     <t>Ask active users (&gt;1 link sent) to rate/review app</t>
   </si>
   <si>
-    <t>Add referral incentive + restart online contest</t>
+    <t>Renew distribution push certificates</t>
+  </si>
+  <si>
+    <t>Week 15</t>
+  </si>
+  <si>
+    <t>Week 16</t>
+  </si>
+  <si>
+    <t>Remove trunk/Examples and build/ folders</t>
+  </si>
+  <si>
+    <t>Capitalize class names</t>
+  </si>
+  <si>
+    <t>Update FB page with contest results</t>
+  </si>
+  <si>
+    <t>Support international users</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1589,8 +1580,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1621,12 +1619,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1637,8 +1629,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2579">
+  <cellStyleXfs count="2597">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4250,10 +4260,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2579">
+  <cellStyles count="2597">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5543,6 +5553,15 @@
     <cellStyle name="Followed Hyperlink" xfId="2574" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2576" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2596" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6832,6 +6851,15 @@
     <cellStyle name="Hyperlink" xfId="2573" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2575" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2577" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2579" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2595" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7164,10 +7192,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E180"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7214,7 +7242,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>298</v>
@@ -7229,15 +7257,15 @@
         <v>26</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="C6" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>118</v>
@@ -7251,7 +7279,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>299</v>
@@ -7265,7 +7293,7 @@
         <v>43</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>284</v>
@@ -7279,7 +7307,7 @@
         <v>290</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -7293,7 +7321,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -7307,7 +7335,7 @@
         <v>287</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -7318,10 +7346,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -7332,16 +7360,16 @@
         <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
       <c r="C14" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -7356,7 +7384,7 @@
         <v>129</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -7370,7 +7398,7 @@
         <v>190</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -7381,7 +7409,7 @@
         <v>29</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -7415,10 +7443,10 @@
         <v>24</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -7429,10 +7457,10 @@
         <v>30</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E21" s="11"/>
     </row>
@@ -7441,7 +7469,7 @@
         <v>286</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E22" s="11"/>
     </row>
@@ -7456,7 +7484,7 @@
         <v>261</v>
       </c>
       <c r="D23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E23" s="9"/>
     </row>
@@ -7468,7 +7496,7 @@
         <v>33</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E24" s="11"/>
     </row>
@@ -7480,10 +7508,10 @@
         <v>53</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E25" s="10"/>
     </row>
@@ -7498,7 +7526,7 @@
         <v>47</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -7512,7 +7540,7 @@
         <v>225</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -7537,7 +7565,7 @@
         <v>154</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -7545,7 +7573,7 @@
         <v>83</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>392</v>
+        <v>426</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -7558,8 +7586,8 @@
       <c r="C31" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="D31" s="30" t="s">
-        <v>350</v>
+      <c r="D31" s="32" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -7572,8 +7600,8 @@
       <c r="C32" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="31" t="s">
-        <v>420</v>
+      <c r="D32" s="30" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -7593,10 +7621,10 @@
         <v>57</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="E34" s="10"/>
     </row>
@@ -7608,10 +7636,10 @@
         <v>58</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>434</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>414</v>
+        <v>425</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>432</v>
       </c>
       <c r="E35" s="12"/>
     </row>
@@ -7622,12 +7650,10 @@
       <c r="B36" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="32" t="s">
-        <v>435</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>432</v>
-      </c>
+      <c r="C36" s="20" t="s">
+        <v>431</v>
+      </c>
+      <c r="D36" s="31"/>
       <c r="E36" s="18"/>
     </row>
     <row r="37" spans="1:5">
@@ -7638,13 +7664,13 @@
         <v>60</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E37" s="10"/>
     </row>
     <row r="38" spans="1:5">
       <c r="C38" s="22" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E38" s="10"/>
     </row>
@@ -7656,7 +7682,7 @@
         <v>63</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E39" s="15"/>
     </row>
@@ -7668,7 +7694,7 @@
         <v>67</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E40" s="16"/>
     </row>
@@ -7689,10 +7715,10 @@
         <v>68</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E42" s="9"/>
     </row>
@@ -7703,11 +7729,11 @@
       <c r="B43" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C43" s="20" t="s">
-        <v>413</v>
+      <c r="C43" s="27" t="s">
+        <v>363</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="E43" s="15"/>
     </row>
@@ -7719,10 +7745,10 @@
         <v>134</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -7732,20 +7758,20 @@
       <c r="B45" t="s">
         <v>135</v>
       </c>
-      <c r="C45" s="27" t="s">
-        <v>376</v>
+      <c r="C45" s="22" t="s">
+        <v>406</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E45" s="15"/>
     </row>
     <row r="46" spans="1:5">
       <c r="C46" s="22" t="s">
-        <v>412</v>
+        <v>364</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="E46" s="15"/>
     </row>
@@ -7757,10 +7783,10 @@
         <v>75</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E47" s="15"/>
     </row>
@@ -7772,7 +7798,7 @@
         <v>77</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -7783,7 +7809,10 @@
         <v>79</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>368</v>
+        <v>370</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -7794,10 +7823,10 @@
         <v>81</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>373</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>320</v>
+        <v>366</v>
+      </c>
+      <c r="D50" s="27" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -7807,11 +7836,11 @@
       <c r="B51" t="s">
         <v>84</v>
       </c>
-      <c r="C51" s="22" t="s">
+      <c r="C51" s="4" t="s">
         <v>369</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>300</v>
+        <v>429</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -7822,10 +7851,10 @@
         <v>100</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -7836,19 +7865,14 @@
         <v>92</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="D53" s="27" t="s">
-        <v>398</v>
+        <v>371</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="C54" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="D54" s="27" t="s">
-        <v>331</v>
-      </c>
+        <v>372</v>
+      </c>
+      <c r="D54" s="4"/>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
@@ -7857,12 +7881,6 @@
       <c r="B55" t="s">
         <v>89</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="D55" s="27" t="s">
-        <v>399</v>
-      </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
@@ -7871,6 +7889,12 @@
       <c r="B56" t="s">
         <v>90</v>
       </c>
+      <c r="C56" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
@@ -7879,6 +7903,12 @@
       <c r="B57" t="s">
         <v>97</v>
       </c>
+      <c r="C57" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
@@ -7887,11 +7917,11 @@
       <c r="B58" t="s">
         <v>99</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>340</v>
+      <c r="C58" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D58" s="27" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -7901,11 +7931,11 @@
       <c r="B59" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C59" s="7" t="s">
-        <v>285</v>
+      <c r="C59" t="s">
+        <v>411</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>316</v>
+        <v>389</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -7915,11 +7945,11 @@
       <c r="B60" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C60" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D60" s="27" t="s">
-        <v>319</v>
+      <c r="C60" t="s">
+        <v>341</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -7930,18 +7960,18 @@
         <v>107</v>
       </c>
       <c r="C61" t="s">
-        <v>419</v>
-      </c>
-      <c r="D61" s="27" t="s">
-        <v>348</v>
+        <v>393</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="C62" t="s">
-        <v>343</v>
-      </c>
-      <c r="D62" s="27" t="s">
-        <v>393</v>
+        <v>352</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -7952,10 +7982,10 @@
         <v>109</v>
       </c>
       <c r="C63" t="s">
-        <v>397</v>
+        <v>353</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>342</v>
+        <v>391</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -7966,10 +7996,10 @@
         <v>111</v>
       </c>
       <c r="C64" t="s">
-        <v>355</v>
-      </c>
-      <c r="D64" s="22" t="s">
-        <v>394</v>
+        <v>273</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -7980,10 +8010,10 @@
         <v>114</v>
       </c>
       <c r="C65" t="s">
-        <v>356</v>
-      </c>
-      <c r="D65" s="22" t="s">
-        <v>318</v>
+        <v>354</v>
+      </c>
+      <c r="D65" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -7994,10 +8024,7 @@
         <v>128</v>
       </c>
       <c r="C66" t="s">
-        <v>273</v>
-      </c>
-      <c r="D66" s="22" t="s">
-        <v>395</v>
+        <v>328</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -8008,10 +8035,7 @@
         <v>116</v>
       </c>
       <c r="C67" t="s">
-        <v>357</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>317</v>
+        <v>402</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -8022,10 +8046,10 @@
         <v>121</v>
       </c>
       <c r="C68" t="s">
-        <v>329</v>
-      </c>
-      <c r="D68" t="s">
-        <v>396</v>
+        <v>304</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -8036,15 +8060,18 @@
         <v>120</v>
       </c>
       <c r="C69" t="s">
-        <v>408</v>
+        <v>422</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="C70" t="s">
-        <v>305</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>224</v>
+        <v>401</v>
+      </c>
+      <c r="D70" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -8055,10 +8082,10 @@
         <v>131</v>
       </c>
       <c r="C71" t="s">
-        <v>430</v>
+        <v>409</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>221</v>
+        <v>346</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -8069,10 +8096,10 @@
         <v>126</v>
       </c>
       <c r="C72" t="s">
-        <v>407</v>
-      </c>
-      <c r="D72" t="s">
-        <v>341</v>
+        <v>410</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -8082,11 +8109,11 @@
       <c r="B73" t="s">
         <v>143</v>
       </c>
-      <c r="C73" t="s">
-        <v>417</v>
+      <c r="C73" s="19" t="s">
+        <v>325</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>349</v>
+        <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -8097,10 +8124,10 @@
         <v>133</v>
       </c>
       <c r="C74" t="s">
-        <v>418</v>
-      </c>
-      <c r="D74" s="19" t="s">
-        <v>228</v>
+        <v>362</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -8110,11 +8137,11 @@
       <c r="B75" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C75" s="19" t="s">
-        <v>326</v>
+      <c r="C75" t="s">
+        <v>405</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>303</v>
+        <v>248</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -8124,12 +8151,6 @@
       <c r="B76" t="s">
         <v>171</v>
       </c>
-      <c r="C76" t="s">
-        <v>365</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>222</v>
-      </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
@@ -8139,10 +8160,12 @@
         <v>172</v>
       </c>
       <c r="C77" t="s">
-        <v>411</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>248</v>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="C78" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -8153,7 +8176,7 @@
         <v>141</v>
       </c>
       <c r="C79" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -8163,9 +8186,6 @@
       <c r="B80" t="s">
         <v>144</v>
       </c>
-      <c r="C80" t="s">
-        <v>272</v>
-      </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
@@ -8175,7 +8195,7 @@
         <v>148</v>
       </c>
       <c r="C81" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -8185,6 +8205,9 @@
       <c r="B82" t="s">
         <v>147</v>
       </c>
+      <c r="C82" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
@@ -8193,8 +8216,8 @@
       <c r="B83" t="s">
         <v>153</v>
       </c>
-      <c r="C83" t="s">
-        <v>291</v>
+      <c r="C83" s="25" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -8204,9 +8227,6 @@
       <c r="B84" t="s">
         <v>151</v>
       </c>
-      <c r="C84" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="13" t="s">
@@ -8215,9 +8235,6 @@
       <c r="B85" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="C85" s="25" t="s">
-        <v>324</v>
-      </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
@@ -8376,7 +8393,7 @@
         <v>197</v>
       </c>
       <c r="B108" s="28" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -8704,10 +8721,10 @@
         <v>7</v>
       </c>
       <c r="B167" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C167" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -8715,130 +8732,140 @@
         <v>6</v>
       </c>
       <c r="B168" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="C168" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B169" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C169" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B170" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="C170" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B171" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C171" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B172" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C172" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B173" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C173" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B174" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C174" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B175" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C175" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B176" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C176" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B177" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="C177" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B178" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="C178" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>416</v>
+        <v>408</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" t="s">
+        <v>428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>